<commit_message>
file in server side maybe... completed but TS is a problem for book
</commit_message>
<xml_diff>
--- a/OralHealth/test.xlsx
+++ b/OralHealth/test.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\js-xlsx-0.11.17\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\OralHealthWeb\OralHealth\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,9 +35,6 @@
     <t>price</t>
   </si>
   <si>
-    <t>apple</t>
-  </si>
-  <si>
     <t>google</t>
   </si>
   <si>
@@ -57,6 +54,9 @@
   </si>
   <si>
     <t>zenphone</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -412,7 +412,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -430,10 +430,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -441,10 +441,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>500</v>
@@ -452,10 +452,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>200</v>
@@ -463,10 +463,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <v>1200</v>

</xml_diff>

<commit_message>
bug bug bug in README
</commit_message>
<xml_diff>
--- a/OralHealth/test.xlsx
+++ b/OralHealth/test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>company</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>zenphone</t>
-  </si>
-  <si>
-    <t>test</t>
   </si>
 </sst>
 </file>
@@ -416,6 +413,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="9.875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -429,14 +429,14 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>10</v>
+      <c r="A2">
+        <v>123456</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2">
-        <v>100</v>
+        <v>123456789</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>